<commit_message>
made report per year(3) and fixed any bugs and create .exe
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -7,8 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="отчёт за Ноябрь(11) 2020" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="отчёт за Октябрь(10) 2020" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="отчёт за 2021 год" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -35,14 +34,6 @@
       <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-    </font>
-    <font>
-      <color rgb="00555555"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <color rgb="00777777"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -66,7 +57,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -75,12 +66,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -448,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,12 +444,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Отчет за месяц работы кабинета реабилитации</t>
+          <t>Отчет за год работы кабинета реабилитации</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Ноябрь 2020г.</t>
+          <t>2021г.</t>
         </is>
       </c>
     </row>
@@ -475,7 +460,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -495,385 +480,147 @@
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>Инопланетянин</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>По отделениям</t>
         </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>КХО</t>
+          <t>реанимация</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>реанимация</t>
+          <t>интенсивного лечения</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>интенсивного лечения</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>По процедурам</t>
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Места</t>
+        </is>
+      </c>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>Исполнители</t>
+        </is>
+      </c>
+    </row>
     <row r="16">
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>Места</t>
-        </is>
-      </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>Исполнители</t>
-        </is>
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Всего</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>Всего</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Всего</t>
+          <t>ТШХ</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>Всего</t>
+          <t>Полковникова Елена Викторовна</t>
         </is>
       </c>
       <c r="K17" s="3" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>ТШХ</t>
+          <t>зал</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>Тест тестовик 11</t>
+          <t>ролдждлорош</t>
         </is>
       </c>
       <c r="K18" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>зал</t>
+          <t>Дурдомовцы</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>Полковникова Елена Викторовна</t>
-        </is>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>Дурдомовцы</t>
+          <t>Нормальные</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
         <v>0</v>
-      </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>пппп</t>
-        </is>
-      </c>
-      <c r="K20" s="3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="inlineStr">
         <is>
-          <t>Нормальные</t>
+          <t>Палата реанимации</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t>Палата реанимации</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" s="5" t="inlineStr">
-        <is>
-          <t>ролдждлорош</t>
-        </is>
-      </c>
-      <c r="K22" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="landscape" paperSize="9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Отчет за месяц работы кабинета реабилитации</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Октябрь 2020г.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Всего человек</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Ребёнок</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>Взрослый</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>удал. категории</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>По отделениям</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>КХО</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>реанимация</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>интенсивного лечения</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>По процедурам</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>Места</t>
-        </is>
-      </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>Исполнители</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>Всего</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>Всего</t>
-        </is>
-      </c>
-      <c r="K17" s="3" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>ТШХ</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3" t="inlineStr">
-        <is>
-          <t>Тест тестовик 11</t>
-        </is>
-      </c>
-      <c r="K18" s="3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>Дурдомовцы</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>Полковникова Елена Викторовна</t>
-        </is>
-      </c>
-      <c r="K19" s="3" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="inlineStr">
-        <is>
-          <t>Нормальные</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>Палата реанимации</t>
-        </is>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t>удал. места</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made report 4 and fixed any bugs
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="отчёт за 2021 год" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="отчёт за день" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="отчёт за период дней" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -627,4 +629,868 @@
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="5"/>
+    <col customWidth="1" max="2" min="2" width="55"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="17"/>
+    <col customWidth="1" max="5" min="5" width="24"/>
+    <col customWidth="1" max="6" min="6" width="7"/>
+    <col customWidth="1" max="7" min="7" width="10"/>
+    <col customWidth="1" max="8" min="8" width="7"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
+    <col customWidth="1" max="10" min="10" width="7"/>
+    <col customWidth="1" max="11" min="11" width="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Журнал работы с пациентами</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>06.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>№ истории</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>взр./реб.</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Отдел</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ffhffhdh 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Всего процедур за 06.01.2021:</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Всего пациентов :</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ……………………………………………………………………………………………………………………………</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Журнал работы с пациентами</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>07.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>№ истории</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>взр./реб.</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>Отдел</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="I23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="J23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ffhffhdh 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>зал</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H24" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+      <c r="J24" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K24" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Всего процедур за 07.01.2021:</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>Всего пациентов :</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>зал……………………………………………………………………………………………………………………………</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" paperSize="9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="5"/>
+    <col customWidth="1" max="2" min="2" width="55"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="17"/>
+    <col customWidth="1" max="5" min="5" width="24"/>
+    <col customWidth="1" max="6" min="6" width="7"/>
+    <col customWidth="1" max="7" min="7" width="10"/>
+    <col customWidth="1" max="8" min="8" width="7"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
+    <col customWidth="1" max="10" min="10" width="7"/>
+    <col customWidth="1" max="11" min="11" width="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Журнал работы с пациентами</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>06.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>№ истории</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>взр./реб.</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Отдел</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ffhffhdh 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H6" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="I6" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+      <c r="J6" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Всего процедур за 06.01.2021:</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Всего пациентов :</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>ТШХ……………………………………………………………………………………………………………………………</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Журнал работы с пациентами</t>
+        </is>
+      </c>
+      <c r="G11" s="1" t="inlineStr">
+        <is>
+          <t>07.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>№ истории</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>взр./реб.</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>Отдел</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ffhffhdh 01.01.2000 </t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Ребёнок</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>КХО</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>зал</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>ПЕВ</t>
+        </is>
+      </c>
+      <c r="H15" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="I15" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>---------</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="inlineStr">
+        <is>
+          <t>-------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Всего процедур за 07.01.2021:</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>Всего пациентов :</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>зал……………………………………………………………………………………………………………………………</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Журнал работы с пациентами</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>08.01.2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>№ истории</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>взр./реб.</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>Отдел</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="G23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="I23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+      <c r="J23" s="2" t="inlineStr">
+        <is>
+          <t>место</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>исп.</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Всего процедур за 08.01.2021:</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>Всего пациентов :</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" paperSize="9"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="10" man="1" max="16383" min="0"/>
+    <brk id="19" man="1" max="16383" min="0"/>
+    <brk id="26" man="1" max="16383" min="0"/>
+  </rowBreaks>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix any bags nd started report_5
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -10,6 +10,7 @@
     <sheet name="отчёт за период дней" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="отчёт за 2021 год" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="отчёт за Январь(01) 2021" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="сборный" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -7101,4 +7102,772 @@
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="1"/>
+    <col customWidth="1" max="2" min="2" width="1"/>
+    <col customWidth="1" max="3" min="3" width="1"/>
+    <col customWidth="1" max="4" min="4" width="1"/>
+    <col customWidth="1" max="5" min="5" width="1"/>
+    <col customWidth="1" max="6" min="6" width="1"/>
+    <col customWidth="1" max="7" min="7" width="1"/>
+    <col customWidth="1" max="8" min="8" width="1"/>
+    <col customWidth="1" max="9" min="9" width="1"/>
+    <col customWidth="1" max="10" min="10" width="1"/>
+    <col customWidth="1" max="11" min="11" width="1"/>
+    <col customWidth="1" max="12" min="12" width="1"/>
+    <col customWidth="1" max="13" min="13" width="1"/>
+    <col customWidth="1" max="14" min="14" width="1"/>
+    <col customWidth="1" max="15" min="15" width="1"/>
+    <col customWidth="1" max="16" min="16" width="1"/>
+    <col customWidth="1" max="17" min="17" width="1"/>
+    <col customWidth="1" max="18" min="18" width="1"/>
+    <col customWidth="1" max="19" min="19" width="1"/>
+    <col customWidth="1" max="20" min="20" width="1"/>
+    <col customWidth="1" max="21" min="21" width="1"/>
+    <col customWidth="1" max="22" min="22" width="1"/>
+    <col customWidth="1" max="23" min="23" width="1"/>
+    <col customWidth="1" max="24" min="24" width="1"/>
+    <col customWidth="1" max="25" min="25" width="1"/>
+    <col customWidth="1" max="26" min="26" width="1"/>
+    <col customWidth="1" max="27" min="27" width="1"/>
+    <col customWidth="1" max="28" min="28" width="1"/>
+    <col customWidth="1" max="29" min="29" width="1"/>
+    <col customWidth="1" max="30" min="30" width="1"/>
+    <col customWidth="1" max="31" min="31" width="1"/>
+    <col customWidth="1" max="32" min="32" width="1"/>
+    <col customWidth="1" max="33" min="33" width="1"/>
+    <col customWidth="1" max="34" min="34" width="1"/>
+    <col customWidth="1" max="35" min="35" width="1"/>
+    <col customWidth="1" max="36" min="36" width="1"/>
+    <col customWidth="1" max="37" min="37" width="1"/>
+    <col customWidth="1" max="38" min="38" width="1"/>
+    <col customWidth="1" max="39" min="39" width="1"/>
+    <col customWidth="1" max="40" min="40" width="1"/>
+    <col customWidth="1" max="41" min="41" width="1"/>
+    <col customWidth="1" max="42" min="42" width="1"/>
+    <col customWidth="1" max="43" min="43" width="1"/>
+    <col customWidth="1" max="44" min="44" width="1"/>
+    <col customWidth="1" max="45" min="45" width="1"/>
+    <col customWidth="1" max="46" min="46" width="1"/>
+    <col customWidth="1" max="47" min="47" width="1"/>
+    <col customWidth="1" max="48" min="48" width="1"/>
+    <col customWidth="1" max="49" min="49" width="1"/>
+    <col customWidth="1" max="50" min="50" width="1"/>
+    <col customWidth="1" max="51" min="51" width="1"/>
+    <col customWidth="1" max="52" min="52" width="1"/>
+    <col customWidth="1" max="53" min="53" width="1"/>
+    <col customWidth="1" max="54" min="54" width="1"/>
+    <col customWidth="1" max="55" min="55" width="1"/>
+    <col customWidth="1" max="56" min="56" width="1"/>
+    <col customWidth="1" max="57" min="57" width="1"/>
+    <col customWidth="1" max="58" min="58" width="1"/>
+    <col customWidth="1" max="59" min="59" width="1"/>
+    <col customWidth="1" max="60" min="60" width="1"/>
+    <col customWidth="1" max="61" min="61" width="1"/>
+    <col customWidth="1" max="62" min="62" width="1"/>
+    <col customWidth="1" max="63" min="63" width="1"/>
+    <col customWidth="1" max="64" min="64" width="1"/>
+    <col customWidth="1" max="65" min="65" width="1"/>
+    <col customWidth="1" max="66" min="66" width="1"/>
+    <col customWidth="1" max="67" min="67" width="1"/>
+    <col customWidth="1" max="68" min="68" width="1"/>
+    <col customWidth="1" max="69" min="69" width="1"/>
+    <col customWidth="1" max="70" min="70" width="1"/>
+    <col customWidth="1" max="71" min="71" width="1"/>
+    <col customWidth="1" max="72" min="72" width="1"/>
+    <col customWidth="1" max="73" min="73" width="1"/>
+    <col customWidth="1" max="74" min="74" width="1"/>
+    <col customWidth="1" max="75" min="75" width="1"/>
+    <col customWidth="1" max="76" min="76" width="1"/>
+    <col customWidth="1" max="77" min="77" width="1"/>
+    <col customWidth="1" max="78" min="78" width="1"/>
+    <col customWidth="1" max="79" min="79" width="1"/>
+    <col customWidth="1" max="80" min="80" width="1"/>
+    <col customWidth="1" max="81" min="81" width="1"/>
+    <col customWidth="1" max="82" min="82" width="1"/>
+    <col customWidth="1" max="83" min="83" width="1"/>
+    <col customWidth="1" max="84" min="84" width="1"/>
+    <col customWidth="1" max="85" min="85" width="1"/>
+    <col customWidth="1" max="86" min="86" width="1"/>
+    <col customWidth="1" max="87" min="87" width="1"/>
+    <col customWidth="1" max="88" min="88" width="1"/>
+    <col customWidth="1" max="89" min="89" width="1"/>
+    <col customWidth="1" max="90" min="90" width="1"/>
+    <col customWidth="1" max="91" min="91" width="1"/>
+    <col customWidth="1" max="92" min="92" width="1"/>
+    <col customWidth="1" max="93" min="93" width="1"/>
+    <col customWidth="1" max="94" min="94" width="1"/>
+    <col customWidth="1" max="95" min="95" width="1"/>
+    <col customWidth="1" max="96" min="96" width="1"/>
+    <col customWidth="1" max="97" min="97" width="1"/>
+    <col customWidth="1" max="98" min="98" width="1"/>
+    <col customWidth="1" max="99" min="99" width="1"/>
+    <col customWidth="1" max="100" min="100" width="1"/>
+    <col customWidth="1" max="101" min="101" width="1"/>
+    <col customWidth="1" max="102" min="102" width="1"/>
+    <col customWidth="1" max="103" min="103" width="1"/>
+    <col customWidth="1" max="104" min="104" width="1"/>
+    <col customWidth="1" max="105" min="105" width="1"/>
+    <col customWidth="1" max="106" min="106" width="1"/>
+    <col customWidth="1" max="107" min="107" width="1"/>
+    <col customWidth="1" max="108" min="108" width="1"/>
+    <col customWidth="1" max="109" min="109" width="1"/>
+    <col customWidth="1" max="110" min="110" width="1"/>
+    <col customWidth="1" max="111" min="111" width="1"/>
+    <col customWidth="1" max="112" min="112" width="1"/>
+    <col customWidth="1" max="113" min="113" width="1"/>
+    <col customWidth="1" max="114" min="114" width="1"/>
+    <col customWidth="1" max="115" min="115" width="1"/>
+    <col customWidth="1" max="116" min="116" width="1"/>
+    <col customWidth="1" max="117" min="117" width="1"/>
+    <col customWidth="1" max="118" min="118" width="1"/>
+    <col customWidth="1" max="119" min="119" width="1"/>
+    <col customWidth="1" max="120" min="120" width="1"/>
+    <col customWidth="1" max="121" min="121" width="1"/>
+    <col customWidth="1" max="122" min="122" width="1"/>
+    <col customWidth="1" max="123" min="123" width="1"/>
+    <col customWidth="1" max="124" min="124" width="1"/>
+    <col customWidth="1" max="125" min="125" width="1"/>
+    <col customWidth="1" max="126" min="126" width="1"/>
+    <col customWidth="1" max="127" min="127" width="1"/>
+    <col customWidth="1" max="128" min="128" width="1"/>
+    <col customWidth="1" max="129" min="129" width="1"/>
+    <col customWidth="1" max="130" min="130" width="1"/>
+    <col customWidth="1" max="131" min="131" width="1"/>
+    <col customWidth="1" max="132" min="132" width="1"/>
+    <col customWidth="1" max="133" min="133" width="1"/>
+    <col customWidth="1" max="134" min="134" width="1"/>
+    <col customWidth="1" max="135" min="135" width="1"/>
+    <col customWidth="1" max="136" min="136" width="1"/>
+    <col customWidth="1" max="137" min="137" width="1"/>
+    <col customWidth="1" max="138" min="138" width="1"/>
+    <col customWidth="1" max="139" min="139" width="1"/>
+    <col customWidth="1" max="140" min="140" width="1"/>
+    <col customWidth="1" max="141" min="141" width="1"/>
+    <col customWidth="1" max="142" min="142" width="1"/>
+    <col customWidth="1" max="143" min="143" width="1"/>
+    <col customWidth="1" max="144" min="144" width="1"/>
+    <col customWidth="1" max="145" min="145" width="1"/>
+    <col customWidth="1" max="146" min="146" width="1"/>
+    <col customWidth="1" max="147" min="147" width="1"/>
+    <col customWidth="1" max="148" min="148" width="1"/>
+    <col customWidth="1" max="149" min="149" width="1"/>
+    <col customWidth="1" max="150" min="150" width="1"/>
+    <col customWidth="1" max="151" min="151" width="1"/>
+    <col customWidth="1" max="152" min="152" width="1"/>
+    <col customWidth="1" max="153" min="153" width="1"/>
+    <col customWidth="1" max="154" min="154" width="1"/>
+    <col customWidth="1" max="155" min="155" width="1"/>
+    <col customWidth="1" max="156" min="156" width="1"/>
+    <col customWidth="1" max="157" min="157" width="1"/>
+    <col customWidth="1" max="158" min="158" width="1"/>
+    <col customWidth="1" max="159" min="159" width="1"/>
+    <col customWidth="1" max="160" min="160" width="1"/>
+    <col customWidth="1" max="161" min="161" width="1"/>
+    <col customWidth="1" max="162" min="162" width="1"/>
+    <col customWidth="1" max="163" min="163" width="1"/>
+    <col customWidth="1" max="164" min="164" width="1"/>
+    <col customWidth="1" max="165" min="165" width="1"/>
+    <col customWidth="1" max="166" min="166" width="1"/>
+    <col customWidth="1" max="167" min="167" width="1"/>
+    <col customWidth="1" max="168" min="168" width="1"/>
+    <col customWidth="1" max="169" min="169" width="1"/>
+    <col customWidth="1" max="170" min="170" width="1"/>
+    <col customWidth="1" max="171" min="171" width="1"/>
+    <col customWidth="1" max="172" min="172" width="1"/>
+    <col customWidth="1" max="173" min="173" width="1"/>
+    <col customWidth="1" max="174" min="174" width="1"/>
+    <col customWidth="1" max="175" min="175" width="1"/>
+    <col customWidth="1" max="176" min="176" width="1"/>
+    <col customWidth="1" max="177" min="177" width="1"/>
+    <col customWidth="1" max="178" min="178" width="1"/>
+    <col customWidth="1" max="179" min="179" width="1"/>
+    <col customWidth="1" max="180" min="180" width="1"/>
+    <col customWidth="1" max="181" min="181" width="1"/>
+    <col customWidth="1" max="182" min="182" width="1"/>
+    <col customWidth="1" max="183" min="183" width="1"/>
+    <col customWidth="1" max="184" min="184" width="1"/>
+    <col customWidth="1" max="185" min="185" width="1"/>
+    <col customWidth="1" max="186" min="186" width="1"/>
+    <col customWidth="1" max="187" min="187" width="1"/>
+    <col customWidth="1" max="188" min="188" width="1"/>
+    <col customWidth="1" max="189" min="189" width="1"/>
+    <col customWidth="1" max="190" min="190" width="1"/>
+    <col customWidth="1" max="191" min="191" width="1"/>
+    <col customWidth="1" max="192" min="192" width="1"/>
+    <col customWidth="1" max="193" min="193" width="1"/>
+    <col customWidth="1" max="194" min="194" width="1"/>
+    <col customWidth="1" max="195" min="195" width="1"/>
+    <col customWidth="1" max="196" min="196" width="1"/>
+    <col customWidth="1" max="197" min="197" width="1"/>
+    <col customWidth="1" max="198" min="198" width="1"/>
+    <col customWidth="1" max="199" min="199" width="1"/>
+    <col customWidth="1" max="200" min="200" width="1"/>
+    <col customWidth="1" max="201" min="201" width="1"/>
+    <col customWidth="1" max="202" min="202" width="1"/>
+    <col customWidth="1" max="203" min="203" width="1"/>
+    <col customWidth="1" max="204" min="204" width="1"/>
+    <col customWidth="1" max="205" min="205" width="1"/>
+    <col customWidth="1" max="206" min="206" width="1"/>
+    <col customWidth="1" max="207" min="207" width="1"/>
+    <col customWidth="1" max="208" min="208" width="1"/>
+    <col customWidth="1" max="209" min="209" width="1"/>
+    <col customWidth="1" max="210" min="210" width="1"/>
+    <col customWidth="1" max="211" min="211" width="1"/>
+    <col customWidth="1" max="212" min="212" width="1"/>
+    <col customWidth="1" max="213" min="213" width="1"/>
+    <col customWidth="1" max="214" min="214" width="1"/>
+    <col customWidth="1" max="215" min="215" width="1"/>
+    <col customWidth="1" max="216" min="216" width="1"/>
+    <col customWidth="1" max="217" min="217" width="1"/>
+    <col customWidth="1" max="218" min="218" width="1"/>
+    <col customWidth="1" max="219" min="219" width="1"/>
+    <col customWidth="1" max="220" min="220" width="1"/>
+    <col customWidth="1" max="221" min="221" width="1"/>
+    <col customWidth="1" max="222" min="222" width="1"/>
+    <col customWidth="1" max="223" min="223" width="1"/>
+    <col customWidth="1" max="224" min="224" width="1"/>
+    <col customWidth="1" max="225" min="225" width="1"/>
+    <col customWidth="1" max="226" min="226" width="1"/>
+    <col customWidth="1" max="227" min="227" width="1"/>
+    <col customWidth="1" max="228" min="228" width="1"/>
+    <col customWidth="1" max="229" min="229" width="1"/>
+    <col customWidth="1" max="230" min="230" width="1"/>
+    <col customWidth="1" max="231" min="231" width="1"/>
+    <col customWidth="1" max="232" min="232" width="1"/>
+    <col customWidth="1" max="233" min="233" width="1"/>
+    <col customWidth="1" max="234" min="234" width="1"/>
+    <col customWidth="1" max="235" min="235" width="1"/>
+    <col customWidth="1" max="236" min="236" width="1"/>
+    <col customWidth="1" max="237" min="237" width="1"/>
+    <col customWidth="1" max="238" min="238" width="1"/>
+    <col customWidth="1" max="239" min="239" width="1"/>
+    <col customWidth="1" max="240" min="240" width="1"/>
+    <col customWidth="1" max="241" min="241" width="1"/>
+    <col customWidth="1" max="242" min="242" width="1"/>
+    <col customWidth="1" max="243" min="243" width="1"/>
+    <col customWidth="1" max="244" min="244" width="1"/>
+    <col customWidth="1" max="245" min="245" width="1"/>
+    <col customWidth="1" max="246" min="246" width="1"/>
+    <col customWidth="1" max="247" min="247" width="1"/>
+    <col customWidth="1" max="248" min="248" width="1"/>
+    <col customWidth="1" max="249" min="249" width="1"/>
+    <col customWidth="1" max="250" min="250" width="1"/>
+    <col customWidth="1" max="251" min="251" width="1"/>
+    <col customWidth="1" max="252" min="252" width="1"/>
+    <col customWidth="1" max="253" min="253" width="1"/>
+    <col customWidth="1" max="254" min="254" width="1"/>
+    <col customWidth="1" max="255" min="255" width="1"/>
+    <col customWidth="1" max="256" min="256" width="1"/>
+    <col customWidth="1" max="257" min="257" width="1"/>
+    <col customWidth="1" max="258" min="258" width="1"/>
+    <col customWidth="1" max="259" min="259" width="1"/>
+    <col customWidth="1" max="260" min="260" width="1"/>
+    <col customWidth="1" max="261" min="261" width="1"/>
+    <col customWidth="1" max="262" min="262" width="1"/>
+    <col customWidth="1" max="263" min="263" width="1"/>
+    <col customWidth="1" max="264" min="264" width="1"/>
+    <col customWidth="1" max="265" min="265" width="1"/>
+    <col customWidth="1" max="266" min="266" width="1"/>
+    <col customWidth="1" max="267" min="267" width="1"/>
+    <col customWidth="1" max="268" min="268" width="1"/>
+    <col customWidth="1" max="269" min="269" width="1"/>
+    <col customWidth="1" max="270" min="270" width="1"/>
+    <col customWidth="1" max="271" min="271" width="1"/>
+    <col customWidth="1" max="272" min="272" width="1"/>
+    <col customWidth="1" max="273" min="273" width="1"/>
+    <col customWidth="1" max="274" min="274" width="1"/>
+    <col customWidth="1" max="275" min="275" width="1"/>
+    <col customWidth="1" max="276" min="276" width="1"/>
+    <col customWidth="1" max="277" min="277" width="1"/>
+    <col customWidth="1" max="278" min="278" width="1"/>
+    <col customWidth="1" max="279" min="279" width="1"/>
+    <col customWidth="1" max="280" min="280" width="1"/>
+    <col customWidth="1" max="281" min="281" width="1"/>
+    <col customWidth="1" max="282" min="282" width="1"/>
+    <col customWidth="1" max="283" min="283" width="1"/>
+    <col customWidth="1" max="284" min="284" width="1"/>
+    <col customWidth="1" max="285" min="285" width="1"/>
+    <col customWidth="1" max="286" min="286" width="1"/>
+    <col customWidth="1" max="287" min="287" width="1"/>
+    <col customWidth="1" max="288" min="288" width="1"/>
+    <col customWidth="1" max="289" min="289" width="1"/>
+    <col customWidth="1" max="290" min="290" width="1"/>
+    <col customWidth="1" max="291" min="291" width="1"/>
+    <col customWidth="1" max="292" min="292" width="1"/>
+    <col customWidth="1" max="293" min="293" width="1"/>
+    <col customWidth="1" max="294" min="294" width="1"/>
+    <col customWidth="1" max="295" min="295" width="1"/>
+    <col customWidth="1" max="296" min="296" width="1"/>
+    <col customWidth="1" max="297" min="297" width="1"/>
+    <col customWidth="1" max="298" min="298" width="1"/>
+    <col customWidth="1" max="299" min="299" width="1"/>
+    <col customWidth="1" max="300" min="300" width="1"/>
+    <col customWidth="1" max="301" min="301" width="1"/>
+    <col customWidth="1" max="302" min="302" width="1"/>
+    <col customWidth="1" max="303" min="303" width="1"/>
+    <col customWidth="1" max="304" min="304" width="1"/>
+    <col customWidth="1" max="305" min="305" width="1"/>
+    <col customWidth="1" max="306" min="306" width="1"/>
+    <col customWidth="1" max="307" min="307" width="1"/>
+    <col customWidth="1" max="308" min="308" width="1"/>
+    <col customWidth="1" max="309" min="309" width="1"/>
+    <col customWidth="1" max="310" min="310" width="1"/>
+    <col customWidth="1" max="311" min="311" width="1"/>
+    <col customWidth="1" max="312" min="312" width="1"/>
+    <col customWidth="1" max="313" min="313" width="1"/>
+    <col customWidth="1" max="314" min="314" width="1"/>
+    <col customWidth="1" max="315" min="315" width="1"/>
+    <col customWidth="1" max="316" min="316" width="1"/>
+    <col customWidth="1" max="317" min="317" width="1"/>
+    <col customWidth="1" max="318" min="318" width="1"/>
+    <col customWidth="1" max="319" min="319" width="1"/>
+    <col customWidth="1" max="320" min="320" width="1"/>
+    <col customWidth="1" max="321" min="321" width="1"/>
+    <col customWidth="1" max="322" min="322" width="1"/>
+    <col customWidth="1" max="323" min="323" width="1"/>
+    <col customWidth="1" max="324" min="324" width="1"/>
+    <col customWidth="1" max="325" min="325" width="1"/>
+    <col customWidth="1" max="326" min="326" width="1"/>
+    <col customWidth="1" max="327" min="327" width="1"/>
+    <col customWidth="1" max="328" min="328" width="1"/>
+    <col customWidth="1" max="329" min="329" width="1"/>
+    <col customWidth="1" max="330" min="330" width="1"/>
+    <col customWidth="1" max="331" min="331" width="1"/>
+    <col customWidth="1" max="332" min="332" width="1"/>
+    <col customWidth="1" max="333" min="333" width="1"/>
+    <col customWidth="1" max="334" min="334" width="1"/>
+    <col customWidth="1" max="335" min="335" width="1"/>
+    <col customWidth="1" max="336" min="336" width="1"/>
+    <col customWidth="1" max="337" min="337" width="1"/>
+    <col customWidth="1" max="338" min="338" width="1"/>
+    <col customWidth="1" max="339" min="339" width="1"/>
+    <col customWidth="1" max="340" min="340" width="1"/>
+    <col customWidth="1" max="341" min="341" width="1"/>
+    <col customWidth="1" max="342" min="342" width="1"/>
+    <col customWidth="1" max="343" min="343" width="1"/>
+    <col customWidth="1" max="344" min="344" width="1"/>
+    <col customWidth="1" max="345" min="345" width="1"/>
+    <col customWidth="1" max="346" min="346" width="1"/>
+    <col customWidth="1" max="347" min="347" width="1"/>
+    <col customWidth="1" max="348" min="348" width="1"/>
+    <col customWidth="1" max="349" min="349" width="1"/>
+    <col customWidth="1" max="350" min="350" width="1"/>
+    <col customWidth="1" max="351" min="351" width="1"/>
+    <col customWidth="1" max="352" min="352" width="1"/>
+    <col customWidth="1" max="353" min="353" width="1"/>
+    <col customWidth="1" max="354" min="354" width="1"/>
+    <col customWidth="1" max="355" min="355" width="1"/>
+    <col customWidth="1" max="356" min="356" width="1"/>
+    <col customWidth="1" max="357" min="357" width="1"/>
+    <col customWidth="1" max="358" min="358" width="1"/>
+    <col customWidth="1" max="359" min="359" width="1"/>
+    <col customWidth="1" max="360" min="360" width="1"/>
+    <col customWidth="1" max="361" min="361" width="1"/>
+    <col customWidth="1" max="362" min="362" width="1"/>
+    <col customWidth="1" max="363" min="363" width="1"/>
+    <col customWidth="1" max="364" min="364" width="1"/>
+    <col customWidth="1" max="365" min="365" width="1"/>
+    <col customWidth="1" max="366" min="366" width="1"/>
+    <col customWidth="1" max="367" min="367" width="1"/>
+    <col customWidth="1" max="368" min="368" width="1"/>
+    <col customWidth="1" max="369" min="369" width="1"/>
+    <col customWidth="1" max="370" min="370" width="1"/>
+    <col customWidth="1" max="371" min="371" width="1"/>
+    <col customWidth="1" max="372" min="372" width="1"/>
+    <col customWidth="1" max="373" min="373" width="1"/>
+    <col customWidth="1" max="374" min="374" width="1"/>
+    <col customWidth="1" max="375" min="375" width="1"/>
+    <col customWidth="1" max="376" min="376" width="1"/>
+    <col customWidth="1" max="377" min="377" width="1"/>
+    <col customWidth="1" max="378" min="378" width="1"/>
+    <col customWidth="1" max="379" min="379" width="1"/>
+    <col customWidth="1" max="380" min="380" width="1"/>
+    <col customWidth="1" max="381" min="381" width="1"/>
+    <col customWidth="1" max="382" min="382" width="1"/>
+    <col customWidth="1" max="383" min="383" width="1"/>
+    <col customWidth="1" max="384" min="384" width="1"/>
+    <col customWidth="1" max="385" min="385" width="1"/>
+    <col customWidth="1" max="386" min="386" width="1"/>
+    <col customWidth="1" max="387" min="387" width="1"/>
+    <col customWidth="1" max="388" min="388" width="1"/>
+    <col customWidth="1" max="389" min="389" width="1"/>
+    <col customWidth="1" max="390" min="390" width="1"/>
+    <col customWidth="1" max="391" min="391" width="1"/>
+    <col customWidth="1" max="392" min="392" width="1"/>
+    <col customWidth="1" max="393" min="393" width="1"/>
+    <col customWidth="1" max="394" min="394" width="1"/>
+    <col customWidth="1" max="395" min="395" width="1"/>
+    <col customWidth="1" max="396" min="396" width="1"/>
+    <col customWidth="1" max="397" min="397" width="1"/>
+    <col customWidth="1" max="398" min="398" width="1"/>
+    <col customWidth="1" max="399" min="399" width="1"/>
+    <col customWidth="1" max="400" min="400" width="1"/>
+    <col customWidth="1" max="401" min="401" width="1"/>
+    <col customWidth="1" max="402" min="402" width="1"/>
+    <col customWidth="1" max="403" min="403" width="1"/>
+    <col customWidth="1" max="404" min="404" width="1"/>
+    <col customWidth="1" max="405" min="405" width="1"/>
+    <col customWidth="1" max="406" min="406" width="1"/>
+    <col customWidth="1" max="407" min="407" width="1"/>
+    <col customWidth="1" max="408" min="408" width="1"/>
+    <col customWidth="1" max="409" min="409" width="1"/>
+    <col customWidth="1" max="410" min="410" width="1"/>
+    <col customWidth="1" max="411" min="411" width="1"/>
+    <col customWidth="1" max="412" min="412" width="1"/>
+    <col customWidth="1" max="413" min="413" width="1"/>
+    <col customWidth="1" max="414" min="414" width="1"/>
+    <col customWidth="1" max="415" min="415" width="1"/>
+    <col customWidth="1" max="416" min="416" width="1"/>
+    <col customWidth="1" max="417" min="417" width="1"/>
+    <col customWidth="1" max="418" min="418" width="1"/>
+    <col customWidth="1" max="419" min="419" width="1"/>
+    <col customWidth="1" max="420" min="420" width="1"/>
+    <col customWidth="1" max="421" min="421" width="1"/>
+    <col customWidth="1" max="422" min="422" width="1"/>
+    <col customWidth="1" max="423" min="423" width="1"/>
+    <col customWidth="1" max="424" min="424" width="1"/>
+    <col customWidth="1" max="425" min="425" width="1"/>
+    <col customWidth="1" max="426" min="426" width="1"/>
+    <col customWidth="1" max="427" min="427" width="1"/>
+    <col customWidth="1" max="428" min="428" width="1"/>
+    <col customWidth="1" max="429" min="429" width="1"/>
+    <col customWidth="1" max="430" min="430" width="1"/>
+    <col customWidth="1" max="431" min="431" width="1"/>
+    <col customWidth="1" max="432" min="432" width="1"/>
+    <col customWidth="1" max="433" min="433" width="1"/>
+    <col customWidth="1" max="434" min="434" width="1"/>
+    <col customWidth="1" max="435" min="435" width="1"/>
+    <col customWidth="1" max="436" min="436" width="1"/>
+    <col customWidth="1" max="437" min="437" width="1"/>
+    <col customWidth="1" max="438" min="438" width="1"/>
+    <col customWidth="1" max="439" min="439" width="1"/>
+    <col customWidth="1" max="440" min="440" width="1"/>
+    <col customWidth="1" max="441" min="441" width="1"/>
+    <col customWidth="1" max="442" min="442" width="1"/>
+    <col customWidth="1" max="443" min="443" width="1"/>
+    <col customWidth="1" max="444" min="444" width="1"/>
+    <col customWidth="1" max="445" min="445" width="1"/>
+    <col customWidth="1" max="446" min="446" width="1"/>
+    <col customWidth="1" max="447" min="447" width="1"/>
+    <col customWidth="1" max="448" min="448" width="1"/>
+    <col customWidth="1" max="449" min="449" width="1"/>
+    <col customWidth="1" max="450" min="450" width="1"/>
+    <col customWidth="1" max="451" min="451" width="1"/>
+    <col customWidth="1" max="452" min="452" width="1"/>
+    <col customWidth="1" max="453" min="453" width="1"/>
+    <col customWidth="1" max="454" min="454" width="1"/>
+    <col customWidth="1" max="455" min="455" width="1"/>
+    <col customWidth="1" max="456" min="456" width="1"/>
+    <col customWidth="1" max="457" min="457" width="1"/>
+    <col customWidth="1" max="458" min="458" width="1"/>
+    <col customWidth="1" max="459" min="459" width="1"/>
+    <col customWidth="1" max="460" min="460" width="1"/>
+    <col customWidth="1" max="461" min="461" width="1"/>
+    <col customWidth="1" max="462" min="462" width="1"/>
+    <col customWidth="1" max="463" min="463" width="1"/>
+    <col customWidth="1" max="464" min="464" width="1"/>
+    <col customWidth="1" max="465" min="465" width="1"/>
+    <col customWidth="1" max="466" min="466" width="1"/>
+    <col customWidth="1" max="467" min="467" width="1"/>
+    <col customWidth="1" max="468" min="468" width="1"/>
+    <col customWidth="1" max="469" min="469" width="1"/>
+    <col customWidth="1" max="470" min="470" width="1"/>
+    <col customWidth="1" max="471" min="471" width="1"/>
+    <col customWidth="1" max="472" min="472" width="1"/>
+    <col customWidth="1" max="473" min="473" width="1"/>
+    <col customWidth="1" max="474" min="474" width="1"/>
+    <col customWidth="1" max="475" min="475" width="1"/>
+    <col customWidth="1" max="476" min="476" width="1"/>
+    <col customWidth="1" max="477" min="477" width="1"/>
+    <col customWidth="1" max="478" min="478" width="1"/>
+    <col customWidth="1" max="479" min="479" width="1"/>
+    <col customWidth="1" max="480" min="480" width="1"/>
+    <col customWidth="1" max="481" min="481" width="1"/>
+    <col customWidth="1" max="482" min="482" width="1"/>
+    <col customWidth="1" max="483" min="483" width="1"/>
+    <col customWidth="1" max="484" min="484" width="1"/>
+    <col customWidth="1" max="485" min="485" width="1"/>
+    <col customWidth="1" max="486" min="486" width="1"/>
+    <col customWidth="1" max="487" min="487" width="1"/>
+    <col customWidth="1" max="488" min="488" width="1"/>
+    <col customWidth="1" max="489" min="489" width="1"/>
+    <col customWidth="1" max="490" min="490" width="1"/>
+    <col customWidth="1" max="491" min="491" width="1"/>
+    <col customWidth="1" max="492" min="492" width="1"/>
+    <col customWidth="1" max="493" min="493" width="1"/>
+    <col customWidth="1" max="494" min="494" width="1"/>
+    <col customWidth="1" max="495" min="495" width="1"/>
+    <col customWidth="1" max="496" min="496" width="1"/>
+    <col customWidth="1" max="497" min="497" width="1"/>
+    <col customWidth="1" max="498" min="498" width="1"/>
+    <col customWidth="1" max="499" min="499" width="1"/>
+    <col customWidth="1" max="500" min="500" width="1"/>
+    <col customWidth="1" max="501" min="501" width="1"/>
+    <col customWidth="1" max="502" min="502" width="1"/>
+    <col customWidth="1" max="503" min="503" width="1"/>
+    <col customWidth="1" max="504" min="504" width="1"/>
+    <col customWidth="1" max="505" min="505" width="1"/>
+    <col customWidth="1" max="506" min="506" width="1"/>
+    <col customWidth="1" max="507" min="507" width="1"/>
+    <col customWidth="1" max="508" min="508" width="1"/>
+    <col customWidth="1" max="509" min="509" width="1"/>
+    <col customWidth="1" max="510" min="510" width="1"/>
+    <col customWidth="1" max="511" min="511" width="1"/>
+    <col customWidth="1" max="512" min="512" width="1"/>
+    <col customWidth="1" max="513" min="513" width="1"/>
+    <col customWidth="1" max="514" min="514" width="1"/>
+    <col customWidth="1" max="515" min="515" width="1"/>
+    <col customWidth="1" max="516" min="516" width="1"/>
+    <col customWidth="1" max="517" min="517" width="1"/>
+    <col customWidth="1" max="518" min="518" width="1"/>
+    <col customWidth="1" max="519" min="519" width="1"/>
+    <col customWidth="1" max="520" min="520" width="1"/>
+    <col customWidth="1" max="521" min="521" width="1"/>
+    <col customWidth="1" max="522" min="522" width="1"/>
+    <col customWidth="1" max="523" min="523" width="1"/>
+    <col customWidth="1" max="524" min="524" width="1"/>
+    <col customWidth="1" max="525" min="525" width="1"/>
+    <col customWidth="1" max="526" min="526" width="1"/>
+    <col customWidth="1" max="527" min="527" width="1"/>
+    <col customWidth="1" max="528" min="528" width="1"/>
+    <col customWidth="1" max="529" min="529" width="1"/>
+    <col customWidth="1" max="530" min="530" width="1"/>
+    <col customWidth="1" max="531" min="531" width="1"/>
+    <col customWidth="1" max="532" min="532" width="1"/>
+    <col customWidth="1" max="533" min="533" width="1"/>
+    <col customWidth="1" max="534" min="534" width="1"/>
+    <col customWidth="1" max="535" min="535" width="1"/>
+    <col customWidth="1" max="536" min="536" width="1"/>
+    <col customWidth="1" max="537" min="537" width="1"/>
+    <col customWidth="1" max="538" min="538" width="1"/>
+    <col customWidth="1" max="539" min="539" width="1"/>
+    <col customWidth="1" max="540" min="540" width="1"/>
+    <col customWidth="1" max="541" min="541" width="1"/>
+    <col customWidth="1" max="542" min="542" width="1"/>
+    <col customWidth="1" max="543" min="543" width="1"/>
+    <col customWidth="1" max="544" min="544" width="1"/>
+    <col customWidth="1" max="545" min="545" width="1"/>
+    <col customWidth="1" max="546" min="546" width="1"/>
+    <col customWidth="1" max="547" min="547" width="1"/>
+    <col customWidth="1" max="548" min="548" width="1"/>
+    <col customWidth="1" max="549" min="549" width="1"/>
+    <col customWidth="1" max="550" min="550" width="1"/>
+    <col customWidth="1" max="551" min="551" width="1"/>
+    <col customWidth="1" max="552" min="552" width="1"/>
+    <col customWidth="1" max="553" min="553" width="1"/>
+    <col customWidth="1" max="554" min="554" width="1"/>
+    <col customWidth="1" max="555" min="555" width="1"/>
+    <col customWidth="1" max="556" min="556" width="1"/>
+    <col customWidth="1" max="557" min="557" width="1"/>
+    <col customWidth="1" max="558" min="558" width="1"/>
+    <col customWidth="1" max="559" min="559" width="1"/>
+    <col customWidth="1" max="560" min="560" width="1"/>
+    <col customWidth="1" max="561" min="561" width="1"/>
+    <col customWidth="1" max="562" min="562" width="1"/>
+    <col customWidth="1" max="563" min="563" width="1"/>
+    <col customWidth="1" max="564" min="564" width="1"/>
+    <col customWidth="1" max="565" min="565" width="1"/>
+    <col customWidth="1" max="566" min="566" width="1"/>
+    <col customWidth="1" max="567" min="567" width="1"/>
+    <col customWidth="1" max="568" min="568" width="1"/>
+    <col customWidth="1" max="569" min="569" width="1"/>
+    <col customWidth="1" max="570" min="570" width="1"/>
+    <col customWidth="1" max="571" min="571" width="1"/>
+    <col customWidth="1" max="572" min="572" width="1"/>
+    <col customWidth="1" max="573" min="573" width="1"/>
+    <col customWidth="1" max="574" min="574" width="1"/>
+    <col customWidth="1" max="575" min="575" width="1"/>
+    <col customWidth="1" max="576" min="576" width="1"/>
+    <col customWidth="1" max="577" min="577" width="1"/>
+    <col customWidth="1" max="578" min="578" width="1"/>
+    <col customWidth="1" max="579" min="579" width="1"/>
+    <col customWidth="1" max="580" min="580" width="1"/>
+    <col customWidth="1" max="581" min="581" width="1"/>
+    <col customWidth="1" max="582" min="582" width="1"/>
+    <col customWidth="1" max="583" min="583" width="1"/>
+    <col customWidth="1" max="584" min="584" width="1"/>
+    <col customWidth="1" max="585" min="585" width="1"/>
+    <col customWidth="1" max="586" min="586" width="1"/>
+    <col customWidth="1" max="587" min="587" width="1"/>
+    <col customWidth="1" max="588" min="588" width="1"/>
+    <col customWidth="1" max="589" min="589" width="1"/>
+    <col customWidth="1" max="590" min="590" width="1"/>
+    <col customWidth="1" max="591" min="591" width="1"/>
+    <col customWidth="1" max="592" min="592" width="1"/>
+    <col customWidth="1" max="593" min="593" width="1"/>
+    <col customWidth="1" max="594" min="594" width="1"/>
+    <col customWidth="1" max="595" min="595" width="1"/>
+    <col customWidth="1" max="596" min="596" width="1"/>
+    <col customWidth="1" max="597" min="597" width="1"/>
+    <col customWidth="1" max="598" min="598" width="1"/>
+    <col customWidth="1" max="599" min="599" width="1"/>
+    <col customWidth="1" max="600" min="600" width="1"/>
+    <col customWidth="1" max="601" min="601" width="1"/>
+    <col customWidth="1" max="602" min="602" width="1"/>
+    <col customWidth="1" max="603" min="603" width="1"/>
+    <col customWidth="1" max="604" min="604" width="1"/>
+    <col customWidth="1" max="605" min="605" width="1"/>
+    <col customWidth="1" max="606" min="606" width="1"/>
+    <col customWidth="1" max="607" min="607" width="1"/>
+    <col customWidth="1" max="608" min="608" width="1"/>
+    <col customWidth="1" max="609" min="609" width="1"/>
+    <col customWidth="1" max="610" min="610" width="1"/>
+    <col customWidth="1" max="611" min="611" width="1"/>
+    <col customWidth="1" max="612" min="612" width="1"/>
+    <col customWidth="1" max="613" min="613" width="1"/>
+    <col customWidth="1" max="614" min="614" width="1"/>
+    <col customWidth="1" max="615" min="615" width="1"/>
+    <col customWidth="1" max="616" min="616" width="1"/>
+    <col customWidth="1" max="617" min="617" width="1"/>
+    <col customWidth="1" max="618" min="618" width="1"/>
+    <col customWidth="1" max="619" min="619" width="1"/>
+    <col customWidth="1" max="620" min="620" width="1"/>
+    <col customWidth="1" max="621" min="621" width="1"/>
+    <col customWidth="1" max="622" min="622" width="1"/>
+    <col customWidth="1" max="623" min="623" width="1"/>
+    <col customWidth="1" max="624" min="624" width="1"/>
+    <col customWidth="1" max="625" min="625" width="1"/>
+    <col customWidth="1" max="626" min="626" width="1"/>
+    <col customWidth="1" max="627" min="627" width="1"/>
+    <col customWidth="1" max="628" min="628" width="1"/>
+    <col customWidth="1" max="629" min="629" width="1"/>
+    <col customWidth="1" max="630" min="630" width="1"/>
+    <col customWidth="1" max="631" min="631" width="1"/>
+    <col customWidth="1" max="632" min="632" width="1"/>
+    <col customWidth="1" max="633" min="633" width="1"/>
+    <col customWidth="1" max="634" min="634" width="1"/>
+    <col customWidth="1" max="635" min="635" width="1"/>
+    <col customWidth="1" max="636" min="636" width="1"/>
+    <col customWidth="1" max="637" min="637" width="1"/>
+    <col customWidth="1" max="638" min="638" width="1"/>
+    <col customWidth="1" max="639" min="639" width="1"/>
+    <col customWidth="1" max="640" min="640" width="1"/>
+    <col customWidth="1" max="641" min="641" width="1"/>
+    <col customWidth="1" max="642" min="642" width="1"/>
+    <col customWidth="1" max="643" min="643" width="1"/>
+    <col customWidth="1" max="644" min="644" width="1"/>
+    <col customWidth="1" max="645" min="645" width="1"/>
+    <col customWidth="1" max="646" min="646" width="1"/>
+    <col customWidth="1" max="647" min="647" width="1"/>
+    <col customWidth="1" max="648" min="648" width="1"/>
+    <col customWidth="1" max="649" min="649" width="1"/>
+    <col customWidth="1" max="650" min="650" width="1"/>
+    <col customWidth="1" max="651" min="651" width="1"/>
+    <col customWidth="1" max="652" min="652" width="1"/>
+    <col customWidth="1" max="653" min="653" width="1"/>
+    <col customWidth="1" max="654" min="654" width="1"/>
+    <col customWidth="1" max="655" min="655" width="1"/>
+    <col customWidth="1" max="656" min="656" width="1"/>
+    <col customWidth="1" max="657" min="657" width="1"/>
+    <col customWidth="1" max="658" min="658" width="1"/>
+    <col customWidth="1" max="659" min="659" width="1"/>
+    <col customWidth="1" max="660" min="660" width="1"/>
+    <col customWidth="1" max="661" min="661" width="1"/>
+    <col customWidth="1" max="662" min="662" width="1"/>
+    <col customWidth="1" max="663" min="663" width="1"/>
+    <col customWidth="1" max="664" min="664" width="1"/>
+    <col customWidth="1" max="665" min="665" width="1"/>
+    <col customWidth="1" max="666" min="666" width="1"/>
+    <col customWidth="1" max="667" min="667" width="1"/>
+    <col customWidth="1" max="668" min="668" width="1"/>
+    <col customWidth="1" max="669" min="669" width="1"/>
+    <col customWidth="1" max="670" min="670" width="1"/>
+    <col customWidth="1" max="671" min="671" width="1"/>
+    <col customWidth="1" max="672" min="672" width="1"/>
+    <col customWidth="1" max="673" min="673" width="1"/>
+    <col customWidth="1" max="674" min="674" width="1"/>
+    <col customWidth="1" max="675" min="675" width="1"/>
+    <col customWidth="1" max="676" min="676" width="1"/>
+    <col customWidth="1" max="677" min="677" width="1"/>
+    <col customWidth="1" max="678" min="678" width="1"/>
+    <col customWidth="1" max="679" min="679" width="1"/>
+    <col customWidth="1" max="680" min="680" width="1"/>
+    <col customWidth="1" max="681" min="681" width="1"/>
+    <col customWidth="1" max="682" min="682" width="1"/>
+    <col customWidth="1" max="683" min="683" width="1"/>
+    <col customWidth="1" max="684" min="684" width="1"/>
+    <col customWidth="1" max="685" min="685" width="1"/>
+    <col customWidth="1" max="686" min="686" width="1"/>
+    <col customWidth="1" max="687" min="687" width="1"/>
+    <col customWidth="1" max="688" min="688" width="1"/>
+    <col customWidth="1" max="689" min="689" width="1"/>
+    <col customWidth="1" max="690" min="690" width="1"/>
+    <col customWidth="1" max="691" min="691" width="1"/>
+    <col customWidth="1" max="692" min="692" width="1"/>
+    <col customWidth="1" max="693" min="693" width="1"/>
+    <col customWidth="1" max="694" min="694" width="1"/>
+    <col customWidth="1" max="695" min="695" width="1"/>
+    <col customWidth="1" max="696" min="696" width="1"/>
+    <col customWidth="1" max="697" min="697" width="1"/>
+    <col customWidth="1" max="698" min="698" width="1"/>
+    <col customWidth="1" max="699" min="699" width="1"/>
+    <col customWidth="1" max="700" min="700" width="1"/>
+    <col customWidth="1" max="701" min="701" width="1"/>
+    <col customWidth="1" max="702" min="702" width="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Сборный отчёт динамики лечения</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>ФИО, год рождения, диагноз</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>№ карты</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>дата с..по..</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>дней лечения</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>дней ЛФК</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>всего процедур</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>сего ед.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" paperSize="9"/>
+</worksheet>
 </file>
</xml_diff>